<commit_message>
Add support for XYZ plot alone in perr_workspace_vol.m, and optional return value from print_calibration.m.
</commit_message>
<xml_diff>
--- a/matlab/testing/template_axis_stats.xlsx
+++ b/matlab/testing/template_axis_stats.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F81EBB-66D9-4199-97BC-A90DC99AF3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC7AE15-6FEF-41E6-A2AE-F8ADB3A24FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21324" yWindow="4056" windowWidth="18456" windowHeight="8916" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5640" yWindow="8676" windowWidth="23136" windowHeight="10620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="by axis" sheetId="1" r:id="rId1"/>
+    <sheet name="combined" sheetId="4" r:id="rId2"/>
+    <sheet name="short" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
   <si>
     <t>On axis</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>RxRyRz</t>
+  </si>
+  <si>
+    <t>RzRyRz</t>
+  </si>
+  <si>
+    <t>RxRyRx</t>
   </si>
 </sst>
 </file>
@@ -473,6 +482,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -518,21 +552,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,27 +559,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XEW28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:H25"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -912,28 +921,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C1" s="91" t="s">
+      <c r="C1" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="85" t="s">
+      <c r="C2" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="86"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="88" t="s">
+      <c r="D2" s="101"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="103" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="90"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="105"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C3" s="42" t="s">
@@ -956,7 +965,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="86" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -982,7 +991,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="92"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1015,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="86" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1032,7 +1041,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="92"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -1056,7 +1065,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="92" t="s">
+      <c r="A8" s="86" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1082,7 +1091,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="92"/>
+      <c r="A9" s="86"/>
       <c r="B9" s="1" t="s">
         <v>4</v>
       </c>
@@ -1106,7 +1115,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="92" t="s">
+      <c r="A10" s="86" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1132,7 +1141,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="92"/>
+      <c r="A11" s="86"/>
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1178,40 +1187,40 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="80"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="82" t="s">
+      <c r="D13" s="95"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="83"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="99"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="91"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="91"/>
+      <c r="D15" s="87"/>
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="37"/>
       <c r="B16" s="37"/>
-      <c r="C16" s="93" t="s">
+      <c r="C16" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="94"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="93" t="s">
+      <c r="D16" s="89"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="94"/>
-      <c r="H16" s="95"/>
+      <c r="G16" s="89"/>
+      <c r="H16" s="90"/>
     </row>
     <row r="17" spans="1:16377" x14ac:dyDescent="0.3">
       <c r="C17" s="54" t="s">
@@ -1234,7 +1243,7 @@
       </c>
     </row>
     <row r="18" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A18" s="92" t="s">
+      <c r="A18" s="86" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1270,7 +1279,7 @@
       <c r="T18" s="13"/>
     </row>
     <row r="19" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A19" s="92"/>
+      <c r="A19" s="86"/>
       <c r="B19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1304,7 +1313,7 @@
       <c r="T19" s="13"/>
     </row>
     <row r="20" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A20" s="92" t="s">
+      <c r="A20" s="86" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1340,7 +1349,7 @@
       <c r="T20" s="13"/>
     </row>
     <row r="21" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A21" s="92"/>
+      <c r="A21" s="86"/>
       <c r="B21" s="1" t="s">
         <v>4</v>
       </c>
@@ -17731,7 +17740,7 @@
       <c r="XEW21" s="13"/>
     </row>
     <row r="22" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A22" s="92" t="s">
+      <c r="A22" s="86" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -17767,7 +17776,7 @@
       <c r="T22" s="13"/>
     </row>
     <row r="23" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A23" s="92"/>
+      <c r="A23" s="86"/>
       <c r="B23" s="1" t="s">
         <v>4</v>
       </c>
@@ -17801,7 +17810,7 @@
       <c r="T23" s="13"/>
     </row>
     <row r="24" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A24" s="92" t="s">
+      <c r="A24" s="86" t="s">
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -34196,7 +34205,7 @@
       <c r="XEW24" s="13"/>
     </row>
     <row r="25" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="A25" s="92"/>
+      <c r="A25" s="86"/>
       <c r="B25" s="1" t="s">
         <v>4</v>
       </c>
@@ -50610,16 +50619,16 @@
       </c>
     </row>
     <row r="27" spans="1:16377" x14ac:dyDescent="0.3">
-      <c r="C27" s="76" t="s">
+      <c r="C27" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="77"/>
-      <c r="E27" s="78"/>
-      <c r="F27" s="76" t="s">
+      <c r="D27" s="92"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="77"/>
-      <c r="H27" s="78"/>
+      <c r="G27" s="92"/>
+      <c r="H27" s="93"/>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
@@ -50645,6 +50654,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:H27"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="C15:H15"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="A18:A19"/>
@@ -50656,13 +50672,6 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:H27"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="C15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -50673,8 +50682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50685,27 +50694,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="100"/>
-      <c r="E1" s="99" t="s">
+      <c r="D1" s="109"/>
+      <c r="E1" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="100"/>
+      <c r="F1" s="109"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C2" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E2" s="75" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -50717,13 +50726,13 @@
       <c r="D3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="96" t="s">
+      <c r="E3" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="97"/>
+      <c r="F3" s="107"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="86" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -50735,7 +50744,7 @@
       <c r="D4" s="7">
         <v>3.3387148766818669E-2</v>
       </c>
-      <c r="E4" s="108">
+      <c r="E4" s="82">
         <v>2.3630683721306842E-3</v>
       </c>
       <c r="F4" s="18">
@@ -50743,7 +50752,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="92"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="1" t="s">
         <v>20</v>
       </c>
@@ -50753,7 +50762,7 @@
       <c r="D5" s="7">
         <v>5.7017248996798019E-2</v>
       </c>
-      <c r="E5" s="108">
+      <c r="E5" s="82">
         <v>5.8901344428600646E-3</v>
       </c>
       <c r="F5" s="18">
@@ -50761,7 +50770,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="86" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -50773,7 +50782,7 @@
       <c r="D6" s="7">
         <v>0.21645641567063875</v>
       </c>
-      <c r="E6" s="108">
+      <c r="E6" s="82">
         <v>2.4858469318971713E-3</v>
       </c>
       <c r="F6" s="18">
@@ -50781,7 +50790,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="92"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
@@ -50791,7 +50800,7 @@
       <c r="D7" s="7">
         <v>0.35312330574928835</v>
       </c>
-      <c r="E7" s="108">
+      <c r="E7" s="82">
         <v>4.4244816246373211E-3</v>
       </c>
       <c r="F7" s="18">
@@ -50799,19 +50808,19 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="92" t="s">
+      <c r="A8" s="86" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="110">
+      <c r="C8" s="84">
         <v>8.3387598978912542E-2</v>
       </c>
       <c r="D8" s="7">
         <v>0.2190161674118101</v>
       </c>
-      <c r="E8" s="108">
+      <c r="E8" s="82">
         <v>3.3967418416973464E-3</v>
       </c>
       <c r="F8" s="18">
@@ -50819,17 +50828,17 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="92"/>
+      <c r="A9" s="86"/>
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="111">
+      <c r="C9" s="85">
         <v>0.14208198444900269</v>
       </c>
       <c r="D9" s="7">
         <v>0.35314821746257236</v>
       </c>
-      <c r="E9" s="109">
+      <c r="E9" s="83">
         <v>6.6668595872414445E-3</v>
       </c>
       <c r="F9" s="18">
@@ -50837,7 +50846,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="92" t="s">
+      <c r="A10" s="86" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -50857,7 +50866,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="92"/>
+      <c r="A11" s="86"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -50908,8 +50917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -50920,27 +50929,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C1" s="99" t="s">
+      <c r="C1" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="100"/>
-      <c r="E1" s="99" t="s">
+      <c r="D1" s="109"/>
+      <c r="E1" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="100"/>
+      <c r="F1" s="109"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C2" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="E2" s="19" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -50952,100 +50961,100 @@
       <c r="D3" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="96" t="s">
+      <c r="E3" s="106" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="97"/>
+      <c r="F3" s="107"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="98" t="s">
+      <c r="A4" s="110" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7">
-        <f>Sheet2!C8</f>
+        <f>combined!C8</f>
         <v>8.3387598978912542E-2</v>
       </c>
       <c r="D4" s="36">
-        <f>Sheet2!D8</f>
+        <f>combined!D8</f>
         <v>0.2190161674118101</v>
       </c>
-      <c r="E4" s="106">
-        <f>Sheet2!E8</f>
+      <c r="E4" s="80">
+        <f>combined!E8</f>
         <v>3.3967418416973464E-3</v>
       </c>
-      <c r="F4" s="107">
-        <f>Sheet2!F8</f>
+      <c r="F4" s="81">
+        <f>combined!F8</f>
         <v>4.961083640517336E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="101"/>
+      <c r="A5" s="111"/>
       <c r="B5" s="29" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="7">
-        <f>Sheet2!C9</f>
+        <f>combined!C9</f>
         <v>0.14208198444900269</v>
       </c>
       <c r="D5" s="36">
-        <f>Sheet2!D9</f>
+        <f>combined!D9</f>
         <v>0.35314821746257236</v>
       </c>
-      <c r="E5" s="106">
-        <f>Sheet2!E9</f>
+      <c r="E5" s="80">
+        <f>combined!E9</f>
         <v>6.6668595872414445E-3</v>
       </c>
-      <c r="F5" s="107">
-        <f>Sheet2!F9</f>
+      <c r="F5" s="81">
+        <f>combined!F9</f>
         <v>6.608934934299847E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="103" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="32">
-        <f>Sheet2!C10</f>
+        <f>combined!C10</f>
         <v>8.4593670992046691E-2</v>
       </c>
       <c r="D6" s="6">
-        <f>Sheet2!D10</f>
+        <f>combined!D10</f>
         <v>9.0372644232087726E-2</v>
       </c>
-      <c r="E6" s="102">
-        <f>Sheet2!E10</f>
+      <c r="E6" s="76">
+        <f>combined!E10</f>
         <v>3.0053565982372855E-3</v>
       </c>
-      <c r="F6" s="103">
-        <f>Sheet2!F10</f>
+      <c r="F6" s="77">
+        <f>combined!F10</f>
         <v>4.7350169134414664E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="98"/>
+      <c r="A7" s="110"/>
       <c r="B7" s="27" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="33">
-        <f>Sheet2!C11</f>
+        <f>combined!C11</f>
         <v>0.1439331744621592</v>
       </c>
       <c r="D7" s="9">
-        <f>Sheet2!D11</f>
+        <f>combined!D11</f>
         <v>0.12558552700725539</v>
       </c>
-      <c r="E7" s="104">
-        <f>Sheet2!E11</f>
+      <c r="E7" s="78">
+        <f>combined!E11</f>
         <v>3.3921988587682053E-3</v>
       </c>
-      <c r="F7" s="105">
-        <f>Sheet2!F11</f>
+      <c r="F7" s="79">
+        <f>combined!F11</f>
         <v>7.2106046816569694E-3</v>
       </c>
     </row>

</xml_diff>